<commit_message>
Update new color scheme for wordcloud + filter out non-verified tweets for sentiment analysis
</commit_message>
<xml_diff>
--- a/snscrape_dataformat.xlsx
+++ b/snscrape_dataformat.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26307"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{134D17C9-F3BD-45A8-88F9-3EF35511519D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Google Drive\My Space\Academic Notes\MSBD 5005\MSBD5005-Project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2C503C-534D-4381-8389-F93038F51175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tweet" sheetId="1" r:id="rId1"/>
@@ -659,7 +664,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -722,7 +727,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1036,14 +1041,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="28.875" customWidth="1"/>
-    <col min="2" max="2" width="52.875" customWidth="1"/>
+    <col min="1" max="1" width="28.88671875" customWidth="1"/>
+    <col min="2" max="2" width="52.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1086,7 +1091,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" ht="15">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1166,7 +1171,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" ht="15">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1182,7 +1187,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" ht="15">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -1190,7 +1195,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" ht="15">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1206,7 +1211,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" ht="15">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -1214,7 +1219,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" ht="15">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -1222,7 +1227,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" ht="15">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -1230,7 +1235,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" ht="15">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -1254,7 +1259,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" ht="15">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -1270,7 +1275,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" ht="15">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -1342,9 +1347,9 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="26.5" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1392,9 +1397,9 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1426,9 +1431,9 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.625" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1488,14 +1493,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD09F908-EFAB-4C1B-9600-0DAAAA37B010}">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="21.375" customWidth="1"/>
-    <col min="2" max="2" width="78.375" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="78.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1538,7 +1543,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" ht="15">
       <c r="A6" t="s">
         <v>76</v>
       </c>
@@ -1626,7 +1631,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" ht="15">
       <c r="A17" t="s">
         <v>90</v>
       </c>
@@ -1650,7 +1655,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" ht="15">
       <c r="A20" t="s">
         <v>94</v>
       </c>
@@ -1703,9 +1708,9 @@
       <selection activeCell="B7" sqref="B7:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17.125" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1753,9 +1758,9 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16.75" customWidth="1"/>
+    <col min="1" max="1" width="16.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">

</xml_diff>